<commit_message>
Add valores de compra e venda
</commit_message>
<xml_diff>
--- a/cotacoes.xlsx
+++ b/cotacoes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,12 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Cotação</t>
+          <t>Compra R$</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Venda R$</t>
         </is>
       </c>
     </row>
@@ -454,6 +459,9 @@
       <c r="B2" t="n">
         <v>5.8335</v>
       </c>
+      <c r="C2" t="n">
+        <v>5.8341</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -464,6 +472,9 @@
       <c r="B3" t="n">
         <v>6.0155</v>
       </c>
+      <c r="C3" t="n">
+        <v>6.0173</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Alteracoes: Agora a consulta é feita via API
</commit_message>
<xml_diff>
--- a/cotacoes.xlsx
+++ b/cotacoes.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,44 +436,45 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Moeda</t>
+          <t>Dolar Compra</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Compra R$</t>
+          <t>Dolar Venda</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Venda R$</t>
+          <t>Euro Compra</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Euro Venda</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Dólar</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>5.8335</v>
-      </c>
-      <c r="C2" t="n">
-        <v>5.8341</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Euro</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>6.0155</v>
-      </c>
-      <c r="C3" t="n">
-        <v>6.0173</v>
+          <t>5.7991</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>5.7991</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>5.7991</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>5.7991</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>